<commit_message>
Documentation to match current database def
</commit_message>
<xml_diff>
--- a/documentation/WLUX_BackEnd_DataDef_Winter2014.xlsx
+++ b/documentation/WLUX_BackEnd_DataDef_Winter2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="848" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="848" firstSheet="3" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="error messages" sheetId="14" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3562" uniqueCount="1466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3562" uniqueCount="1467">
   <si>
     <t>recordSeq</t>
   </si>
@@ -4152,9 +4152,6 @@
     <t>relational link to study id</t>
   </si>
   <si>
-    <t>studyMeasureId (was recordSeq)</t>
-  </si>
-  <si>
     <t>Primary key -- This table holds Independent Variables. Each record in this table has a one to many relation with study_variations which holds the LEVELS for each IV in this table</t>
   </si>
   <si>
@@ -4432,6 +4429,12 @@
   </si>
   <si>
     <t xml:space="preserve">type </t>
+  </si>
+  <si>
+    <t>Just to name a few... Each ENUM will have its own computation and validation algorithm</t>
+  </si>
+  <si>
+    <t>studyMeasureId</t>
   </si>
 </sst>
 </file>
@@ -5002,13 +5005,13 @@
         <v>1257</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5022,7 +5025,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>1284</v>
@@ -5046,7 +5049,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="9" t="s">
@@ -5068,7 +5071,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="9" t="s">
@@ -5087,10 +5090,10 @@
         <v>1282</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="9" t="s">
@@ -5109,10 +5112,10 @@
         <v>1283</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="9" t="s">
@@ -5178,13 +5181,13 @@
         <v>1257</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5198,7 +5201,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>1284</v>
@@ -5207,7 +5210,7 @@
         <v>1330</v>
       </c>
       <c r="H2" s="18" t="str">
-        <f t="shared" ref="H2:H20" si="0">CONCATENATE("  ",A2," ", B2, " ", C2," ", D2," ",E2," COMMENT '",SUBSTITUTE(F2,"'",""),"',")</f>
+        <f t="shared" ref="H2:H19" si="0">CONCATENATE("  ",A2," ", B2, " ", C2," ", D2," ",E2," COMMENT '",SUBSTITUTE(F2,"'",""),"',")</f>
         <v xml:space="preserve">  studyStepId bigint(20) unsigned NOT NULL AUTO_INCREMENT COMMENT 'Unique record ID',</v>
       </c>
     </row>
@@ -5222,11 +5225,11 @@
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="H3" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5235,7 +5238,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -5244,11 +5247,11 @@
         <v>2</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="H4" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5257,20 +5260,20 @@
     </row>
     <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="H5" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5279,20 +5282,20 @@
     </row>
     <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="H6" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5301,20 +5304,20 @@
     </row>
     <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="H7" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5323,20 +5326,20 @@
     </row>
     <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="H8" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5352,10 +5355,10 @@
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="H9" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5370,14 +5373,14 @@
         <v>8</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F10" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="H10" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5386,20 +5389,20 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F11" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="H11" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5414,14 +5417,14 @@
         <v>5</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F12" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="H12" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5436,14 +5439,14 @@
         <v>5</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F13" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="H13" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5458,14 +5461,14 @@
         <v>5</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F14" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="H14" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5474,20 +5477,20 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F15" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="H15" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5496,20 +5499,20 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="H16" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5518,20 +5521,20 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="H17" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5540,20 +5543,20 @@
     </row>
     <row r="18" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="H18" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5568,7 +5571,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E19" s="21"/>
       <c r="F19" s="18" t="s">
@@ -5587,16 +5590,16 @@
         <v>10</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="H20" s="18" t="str">
-        <f t="shared" ref="H19:H20" si="1">CONCATENATE("  ",A20," ", B20, " ", C20," ", D20," ",E20," COMMENT '",SUBSTITUTE(F20,"'",""),"',")</f>
+        <f t="shared" ref="H20" si="1">CONCATENATE("  ",A20," ", B20, " ", C20," ", D20," ",E20," COMMENT '",SUBSTITUTE(F20,"'",""),"',")</f>
         <v xml:space="preserve">  dateModified timestamp  NOT NULL DEFAULT CURRENT_TIMESTAMP ON UPDATE CURRENT_TIMESTAMP  COMMENT 'The date the record was updated in server local time.',</v>
       </c>
     </row>
@@ -5643,13 +5646,13 @@
         <v>1257</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5663,22 +5666,22 @@
         <v>2</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>1284</v>
       </c>
       <c r="F2" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="H2" s="18" t="str">
-        <f t="shared" ref="H2:H9" si="0">CONCATENATE("  ",A2," ", B2, " ", C2," ", D2," ",E2," COMMENT '",SUBSTITUTE(F2,"'",""),"',")</f>
+        <f t="shared" ref="H2:H8" si="0">CONCATENATE("  ",A2," ", B2, " ", C2," ", D2," ",E2," COMMENT '",SUBSTITUTE(F2,"'",""),"',")</f>
         <v xml:space="preserve">  studyVariationId bigint(20) unsigned NOT NULL AUTO_INCREMENT COMMENT 'Unique record ID of this variation',</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -5687,11 +5690,11 @@
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="H3" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5706,14 +5709,14 @@
         <v>33</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="H4" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5722,20 +5725,20 @@
     </row>
     <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="H5" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5751,7 +5754,7 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="21" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="F6" t="s">
         <v>1226</v>
@@ -5769,10 +5772,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" t="s">
@@ -5791,7 +5794,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="18" t="s">
@@ -5810,16 +5813,16 @@
         <v>10</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="H9" s="18" t="str">
-        <f t="shared" ref="H8:H9" si="1">CONCATENATE("  ",A9," ", B9, " ", C9," ", D9," ",E9," COMMENT '",SUBSTITUTE(F9,"'",""),"',")</f>
+        <f t="shared" ref="H9" si="1">CONCATENATE("  ",A9," ", B9, " ", C9," ", D9," ",E9," COMMENT '",SUBSTITUTE(F9,"'",""),"',")</f>
         <v xml:space="preserve">  dateModified timestamp  NOT NULL DEFAULT CURRENT_TIMESTAMP ON UPDATE CURRENT_TIMESTAMP  COMMENT 'The date the record was updated in server local time.',</v>
       </c>
     </row>
@@ -5837,7 +5840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H18"/>
     </sheetView>
   </sheetViews>
@@ -5860,13 +5863,13 @@
         <v>1257</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5880,7 +5883,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>1284</v>
@@ -5889,7 +5892,7 @@
         <v>1265</v>
       </c>
       <c r="H2" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5900,14 +5903,14 @@
         <v>33</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="H3" s="18" t="str">
         <f t="shared" ref="H3:H17" si="0">CONCATENATE("  ",A3," ", B3, " ", C3," ", D3," ",E3," COMMENT '",SUBSTITUTE(F3,"'",""),"',")</f>
@@ -5925,7 +5928,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" t="s">
@@ -5944,10 +5947,10 @@
         <v>1278</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>1258</v>
@@ -5965,14 +5968,14 @@
         <v>33</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="H6" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5987,13 +5990,13 @@
         <v>33</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F7" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="H7" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6008,13 +6011,13 @@
         <v>33</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F8" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="H8" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6029,13 +6032,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F9" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="H9" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6050,14 +6053,14 @@
         <v>5</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="H10" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6073,7 +6076,7 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="21" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="F11" t="s">
         <v>1268</v>
@@ -6091,10 +6094,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" t="s">
@@ -6113,10 +6116,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" t="s">
@@ -6135,14 +6138,14 @@
         <v>5</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E14" s="19"/>
       <c r="F14" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="H14" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6157,14 +6160,14 @@
         <v>5</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="H15" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6176,19 +6179,19 @@
         <v>50</v>
       </c>
       <c r="B16" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1412</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>1458</v>
       </c>
-      <c r="C16" t="s">
-        <v>1440</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1413</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>1459</v>
-      </c>
       <c r="F16" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="H16" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6203,7 +6206,7 @@
         <v>27</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="18" t="s">
@@ -6222,16 +6225,16 @@
         <v>10</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="H18" s="18" t="str">
-        <f t="shared" ref="H17:H18" si="1">CONCATENATE("  ",A18," ", B18, " ", C18," ", D18," ",E18," COMMENT '",SUBSTITUTE(F18,"'",""),"',")</f>
+        <f t="shared" ref="H18" si="1">CONCATENATE("  ",A18," ", B18, " ", C18," ", D18," ",E18," COMMENT '",SUBSTITUTE(F18,"'",""),"',")</f>
         <v xml:space="preserve">  dateModified timestamp  NOT NULL DEFAULT CURRENT_TIMESTAMP ON UPDATE CURRENT_TIMESTAMP  COMMENT 'The date the record was updated in server local time.',</v>
       </c>
     </row>
@@ -6251,7 +6254,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H11" sqref="H2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6278,18 +6281,18 @@
         <v>1255</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1372</v>
+        <v>1466</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -6298,7 +6301,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>1284</v>
@@ -6308,7 +6311,7 @@
       </c>
       <c r="H2" s="18" t="str">
         <f>CONCATENATE("  ",A2," ", B2, " ", C2," ", D2," ",E2," COMMENT '",SUBSTITUTE(F2,"'",""),"',")</f>
-        <v xml:space="preserve">  studyMeasureId (was recordSeq) bigint(20) unsigned NOT NULL AUTO_INCREMENT COMMENT 'primary key',</v>
+        <v xml:space="preserve">  studyMeasureId bigint(20) unsigned NOT NULL AUTO_INCREMENT COMMENT 'primary key',</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6322,7 +6325,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F3" t="s">
         <v>1371</v>
@@ -6334,7 +6337,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -6343,10 +6346,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F4" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="H4" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6361,14 +6364,14 @@
         <v>1234</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F5" t="s">
-        <v>1244</v>
+        <v>1465</v>
       </c>
       <c r="H5" s="18" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  variableType enum('participantCount','taskTime')  NOT NULL  COMMENT 'Just to name a few… Each ENUM will have its own computation and validation algorithm',</v>
+        <v xml:space="preserve">  variableType enum('participantCount','taskTime')  NOT NULL  COMMENT 'Just to name a few... Each ENUM will have its own computation and validation algorithm',</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6379,7 +6382,7 @@
         <v>1236</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F6" t="s">
         <v>1238</v>
@@ -6397,10 +6400,10 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F7" t="s">
         <v>1239</v>
@@ -6418,10 +6421,10 @@
         <v>1241</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F8" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="H8" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6436,10 +6439,10 @@
         <v>1241</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F9" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="H9" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6454,7 +6457,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="18" t="s">
@@ -6473,13 +6476,13 @@
         <v>10</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="H11" s="18" t="str">
         <f t="shared" ref="H11" si="1">CONCATENATE("  ",A11," ", B11, " ", C11," ", D11," ",E11," COMMENT '",SUBSTITUTE(F11,"'",""),"',")</f>
@@ -6496,7 +6499,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6523,18 +6526,18 @@
         <v>1257</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -6543,16 +6546,16 @@
         <v>2</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>1284</v>
       </c>
       <c r="F2" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="H2" s="18" t="str">
-        <f t="shared" ref="H2:H6" si="0">CONCATENATE("  ",A2," ", B2, " ", C2," ", D2," ",E2," COMMENT '",SUBSTITUTE(F2,"'",""),"',")</f>
+        <f t="shared" ref="H2:H5" si="0">CONCATENATE("  ",A2," ", B2, " ", C2," ", D2," ",E2," COMMENT '",SUBSTITUTE(F2,"'",""),"',")</f>
         <v xml:space="preserve">  studyVariableId bigint(20) unsigned NOT NULL AUTO_INCREMENT COMMENT 'Primary key -- This table holds Independent Variables. Each record in this table has a one to many relation with study_variations which holds the LEVELS for each IV in this table',</v>
       </c>
     </row>
@@ -6567,10 +6570,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F3" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="H3" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6579,19 +6582,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F4" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="H4" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6606,7 +6609,7 @@
         <v>27</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E5" s="21"/>
       <c r="F5" s="18" t="s">
@@ -6625,16 +6628,16 @@
         <v>10</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="H6" s="18" t="str">
-        <f t="shared" ref="H5:H6" si="1">CONCATENATE("  ",A6," ", B6, " ", C6," ", D6," ",E6," COMMENT '",SUBSTITUTE(F6,"'",""),"',")</f>
+        <f t="shared" ref="H6" si="1">CONCATENATE("  ",A6," ", B6, " ", C6," ", D6," ",E6," COMMENT '",SUBSTITUTE(F6,"'",""),"',")</f>
         <v xml:space="preserve">  dateModified timestamp  NOT NULL DEFAULT CURRENT_TIMESTAMP ON UPDATE CURRENT_TIMESTAMP  COMMENT 'The date the record was updated in server local time.',</v>
       </c>
     </row>
@@ -6647,8 +6650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H2:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6675,13 +6678,13 @@
         <v>1257</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6695,7 +6698,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>1284</v>
@@ -6719,7 +6722,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F3" t="s">
         <v>1369</v>
@@ -6734,10 +6737,10 @@
         <v>1365</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="14" t="s">
@@ -6759,7 +6762,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F5" t="s">
         <v>1367</v>
@@ -18673,13 +18676,13 @@
         <v>1257</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -18693,7 +18696,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>1284</v>
@@ -18714,10 +18717,10 @@
         <v>33</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="11" t="s">
@@ -18736,10 +18739,10 @@
         <v>33</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="11" t="s">
@@ -18755,13 +18758,13 @@
         <v>1261</v>
       </c>
       <c r="B5" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="D5" s="20" t="s">
+        <v>1459</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>1460</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>1461</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>1315</v>
@@ -18776,13 +18779,13 @@
         <v>1262</v>
       </c>
       <c r="B6" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="D6" s="20" t="s">
+        <v>1459</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>1460</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>1461</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>1316</v>
@@ -18831,13 +18834,13 @@
         <v>1257</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -18851,7 +18854,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>1284</v>
@@ -18860,7 +18863,7 @@
         <v>1312</v>
       </c>
       <c r="H2" s="18" t="str">
-        <f t="shared" ref="H2:H8" si="0">CONCATENATE("  ",A2," ", B2, " ", C2," ", D2," ",E2," COMMENT '",SUBSTITUTE(F2,"'",""),"',")</f>
+        <f t="shared" ref="H2:H7" si="0">CONCATENATE("  ",A2," ", B2, " ", C2," ", D2," ",E2," COMMENT '",SUBSTITUTE(F2,"'",""),"',")</f>
         <v xml:space="preserve">  gratuityLogId bigint(20) unsigned NOT NULL  AUTO_INCREMENT COMMENT 'Unique record ID.',</v>
       </c>
     </row>
@@ -18875,7 +18878,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="12" t="s">
@@ -18894,11 +18897,11 @@
         <v>33</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>1320</v>
@@ -18916,10 +18919,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>1318</v>
@@ -18937,10 +18940,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>1319</v>
@@ -18958,7 +18961,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E7" s="21"/>
       <c r="F7" s="18" t="s">
@@ -18977,16 +18980,16 @@
         <v>10</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="H8" s="18" t="str">
-        <f t="shared" ref="H7:H8" si="1">CONCATENATE("  ",A8," ", B8, " ", C8," ", D8," ",E8," COMMENT '",SUBSTITUTE(F8,"'",""),"',")</f>
+        <f t="shared" ref="H8" si="1">CONCATENATE("  ",A8," ", B8, " ", C8," ", D8," ",E8," COMMENT '",SUBSTITUTE(F8,"'",""),"',")</f>
         <v xml:space="preserve">  dateModified timestamp  NOT NULL DEFAULT CURRENT_TIMESTAMP ON UPDATE CURRENT_TIMESTAMP  COMMENT 'The date the record was updated in server local time.',</v>
       </c>
     </row>
@@ -19029,13 +19032,13 @@
         <v>1257</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -19049,7 +19052,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>1284</v>
@@ -19071,10 +19074,10 @@
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="20" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="F3" t="s">
         <v>1329</v>
@@ -19095,7 +19098,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F4" t="s">
         <v>1321</v>
@@ -19113,10 +19116,10 @@
         <v>13</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" t="s">
@@ -19138,7 +19141,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" t="s">
@@ -19160,11 +19163,11 @@
         <v>2</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="H7" s="18" t="str">
         <f t="shared" si="0"/>
@@ -19173,7 +19176,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -19182,11 +19185,11 @@
         <v>2</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="H8" s="18" t="str">
         <f t="shared" si="0"/>
@@ -19204,11 +19207,11 @@
         <v>2</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="H9" s="18" t="str">
         <f t="shared" si="0"/>
@@ -19223,10 +19226,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F10" t="s">
         <v>1324</v>
@@ -19244,10 +19247,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F11" t="s">
         <v>1325</v>
@@ -19265,10 +19268,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F12" t="s">
         <v>1326</v>
@@ -19286,10 +19289,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F13" t="s">
         <v>1327</v>
@@ -19307,10 +19310,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F14" t="s">
         <v>1328</v>
@@ -19379,13 +19382,13 @@
         <v>1257</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -19399,7 +19402,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>1284</v>
@@ -19423,10 +19426,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>1412</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>1413</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>1414</v>
       </c>
       <c r="F3" t="s">
         <v>1337</v>
@@ -19447,10 +19450,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>1412</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>1413</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>1414</v>
       </c>
       <c r="F4" t="s">
         <v>1331</v>
@@ -19471,13 +19474,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="15" t="s">
+        <v>1412</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>1413</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>1414</v>
-      </c>
       <c r="F5" s="14" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="H5" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19486,7 +19489,7 @@
     </row>
     <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>16</v>
@@ -19495,13 +19498,13 @@
         <v>2</v>
       </c>
       <c r="D6" s="15" t="s">
+        <v>1412</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>1413</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>1414</v>
-      </c>
       <c r="F6" s="14" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="H6" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19510,20 +19513,20 @@
     </row>
     <row r="7" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="H7" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19532,20 +19535,20 @@
     </row>
     <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="H8" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19554,20 +19557,20 @@
     </row>
     <row r="9" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="H9" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19576,20 +19579,20 @@
     </row>
     <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="H10" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19605,10 +19608,10 @@
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="H11" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19623,14 +19626,14 @@
         <v>8</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="H12" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19639,20 +19642,20 @@
     </row>
     <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="H13" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19667,14 +19670,14 @@
         <v>5</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="H14" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19689,14 +19692,14 @@
         <v>5</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="H15" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19711,14 +19714,14 @@
         <v>5</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="H16" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19727,20 +19730,20 @@
     </row>
     <row r="17" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="H17" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19749,20 +19752,20 @@
     </row>
     <row r="18" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="H18" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19771,20 +19774,20 @@
     </row>
     <row r="19" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="H19" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19793,20 +19796,20 @@
     </row>
     <row r="20" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="H20" s="14" t="str">
         <f t="shared" si="0"/>
@@ -19821,7 +19824,7 @@
         <v>27</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" t="s">
@@ -19840,10 +19843,10 @@
         <v>10</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="F22" t="s">
         <v>1335</v>
@@ -19947,18 +19950,18 @@
         <v>1257</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>1</v>
@@ -19967,7 +19970,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>1284</v>
@@ -19991,10 +19994,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="H3" s="14" t="str">
         <f t="shared" ref="H3:H5" si="0">CONCATENATE("  ",A3," ", B3, " ", C3," ", D3," ",E3," COMMENT '",SUBSTITUTE(F3,"'",""),"',")</f>
@@ -20006,10 +20009,10 @@
         <v>1365</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>1368</v>
@@ -20030,7 +20033,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>1367</v>
@@ -20078,18 +20081,18 @@
         <v>1257</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>35</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -20098,7 +20101,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>1284</v>
@@ -20122,7 +20125,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="13" t="s">
@@ -20144,7 +20147,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="13" t="s">
@@ -20166,7 +20169,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="13" t="s">
@@ -20188,7 +20191,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="13" t="s">
@@ -20210,11 +20213,11 @@
         <v>2</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="13" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="H7" s="18" t="str">
         <f t="shared" si="0"/>
@@ -20229,7 +20232,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="13" t="s">
@@ -20248,7 +20251,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="13" t="s">
@@ -20267,7 +20270,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="18" t="s">
@@ -20286,16 +20289,16 @@
         <v>10</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>1335</v>
       </c>
       <c r="H11" s="18" t="str">
-        <f t="shared" ref="H10:H11" si="1">CONCATENATE("  ",A11," ", B11, " ", C11," ", D11," ",E11," COMMENT '",SUBSTITUTE(F11,"'",""),"',")</f>
+        <f t="shared" ref="H11" si="1">CONCATENATE("  ",A11," ", B11, " ", C11," ", D11," ",E11," COMMENT '",SUBSTITUTE(F11,"'",""),"',")</f>
         <v xml:space="preserve">  dateModified timestamp  NOT NULL DEFAULT CURRENT_TIMESTAMP ON UPDATE CURRENT_TIMESTAMP  COMMENT 'The date the record was created in server local time.',</v>
       </c>
     </row>
@@ -20335,13 +20338,13 @@
         <v>1257</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -20355,7 +20358,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>1284</v>
@@ -20379,7 +20382,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="14" t="s">
@@ -20398,11 +20401,11 @@
         <v>41</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>1347</v>
@@ -20420,11 +20423,11 @@
         <v>25</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>1348</v>
@@ -20442,11 +20445,11 @@
         <v>5</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>1349</v>
@@ -20464,11 +20467,11 @@
         <v>33</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>1350</v>
@@ -20486,11 +20489,11 @@
         <v>33</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>1351</v>
@@ -20508,11 +20511,11 @@
         <v>5</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>1352</v>
@@ -20524,17 +20527,17 @@
     </row>
     <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>1353</v>
@@ -20546,17 +20549,17 @@
     </row>
     <row r="11" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>1354</v>
@@ -20571,19 +20574,19 @@
         <v>50</v>
       </c>
       <c r="B12" s="18" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>1412</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>1458</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>1440</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>1413</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>1459</v>
-      </c>
       <c r="F12" s="18" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="H12" s="18" t="str">
         <f t="shared" si="0"/>
@@ -20599,7 +20602,7 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="17" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>1355</v>
@@ -20618,7 +20621,7 @@
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="17" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>1356</v>
@@ -20636,10 +20639,10 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="14" t="s">
@@ -20659,7 +20662,7 @@
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="17" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>1358</v>
@@ -20677,10 +20680,10 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="14" t="s">
@@ -20699,11 +20702,11 @@
         <v>5</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>1332</v>
@@ -20721,11 +20724,11 @@
         <v>5</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>1333</v>
@@ -20743,11 +20746,11 @@
         <v>5</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>1334</v>
@@ -20766,7 +20769,7 @@
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="17" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>1360</v>
@@ -20785,7 +20788,7 @@
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="17" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>1361</v>
@@ -20803,7 +20806,7 @@
         <v>27</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="14" t="s">
@@ -20822,10 +20825,10 @@
         <v>10</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>1335</v>
@@ -20870,13 +20873,13 @@
         <v>1257</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -20890,7 +20893,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>1284</v>
@@ -20914,11 +20917,11 @@
         <v>2</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="18" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="H3" s="14" t="str">
         <f t="shared" si="0"/>
@@ -20933,14 +20936,14 @@
         <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="18" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="H4" s="14" t="str">
         <f t="shared" si="0"/>
@@ -20955,14 +20958,14 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="16" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="H5" s="14" t="str">
         <f t="shared" si="0"/>
@@ -20981,10 +20984,10 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="16" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="H6" s="14" t="str">
         <f t="shared" si="0"/>
@@ -20999,11 +21002,11 @@
         <v>27</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="18" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="H7" s="14" t="str">
         <f t="shared" si="0"/>
@@ -21018,11 +21021,11 @@
         <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="18" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="H8" s="14" t="str">
         <f t="shared" si="0"/>
@@ -21037,14 +21040,14 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="16" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="H9" s="14" t="str">
         <f t="shared" si="0"/>
@@ -21059,14 +21062,14 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="16" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="H10" s="14" t="str">
         <f t="shared" si="0"/>
@@ -21082,10 +21085,10 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="17" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="H11" s="14" t="str">
         <f t="shared" si="0"/>
@@ -21101,7 +21104,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="17" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="F12" t="s">
         <v>1231</v>
@@ -21116,16 +21119,16 @@
         <v>1294</v>
       </c>
       <c r="B13" s="18" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>1412</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>1458</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>1440</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>1413</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>1459</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>1223</v>
@@ -21143,7 +21146,7 @@
         <v>27</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="14" t="s">
@@ -21162,16 +21165,16 @@
         <v>10</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="H15" s="14" t="str">
-        <f t="shared" ref="H14:H15" si="1">CONCATENATE("  ",A15," ", B15, " ", C15," ", D15," ",E15," COMMENT '",SUBSTITUTE(F15,"'",""),"',")</f>
+        <f t="shared" ref="H15" si="1">CONCATENATE("  ",A15," ", B15, " ", C15," ", D15," ",E15," COMMENT '",SUBSTITUTE(F15,"'",""),"',")</f>
         <v xml:space="preserve">  dateModified timestamp  NOT NULL DEFAULT CURRENT_TIMESTAMP ON UPDATE CURRENT_TIMESTAMP  COMMENT 'The date the record was updated in server local time.',</v>
       </c>
     </row>

</xml_diff>